<commit_message>
Added new features and fixed bugs
</commit_message>
<xml_diff>
--- a/data/DigitalTwin.xlsx
+++ b/data/DigitalTwin.xlsx
@@ -1,34 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_1A914465CA64B1F1CBB654FC0B496ED4631155BB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kota.kiran\OneDrive\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83353050-76DB-45E8-801F-49C36332AF42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3980" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Store" sheetId="1" r:id="rId1"/>
     <sheet name="warehouse" sheetId="2" r:id="rId2"/>
-    <sheet name="warehouse_demand" sheetId="3" r:id="rId3"/>
+    <sheet name="warehouse_inventory" sheetId="3" r:id="rId3"/>
     <sheet name="Store_inventory" sheetId="4" r:id="rId4"/>
     <sheet name="item_capacity" sheetId="5" r:id="rId5"/>
+    <sheet name="Cost" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
     <ext uri="GoogleSheetsCustomDataVersion2">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="ele+BmCRBDINDvZGaYLsMH1semQ0RbfHTIXgDEhYdI0="/>
@@ -38,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="15">
   <si>
     <t>Item</t>
   </si>
@@ -75,16 +70,32 @@
   <si>
     <t>Capacity</t>
   </si>
+  <si>
+    <t>Inventory Carrying cost</t>
+  </si>
+  <si>
+    <t>Shipping cost</t>
+  </si>
+  <si>
+    <t>Fluctuation</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -123,7 +134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -183,34 +194,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,13 +463,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -445,8 +481,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -456,8 +495,11 @@
       <c r="C2" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -467,8 +509,11 @@
       <c r="C3" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -478,8 +523,11 @@
       <c r="C4" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -489,8 +537,11 @@
       <c r="C5" s="1">
         <v>33</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -500,8 +551,11 @@
       <c r="C6" s="1">
         <v>80</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -511,8 +565,11 @@
       <c r="C7" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -522,8 +579,11 @@
       <c r="C8" s="1">
         <v>45</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>4</v>
       </c>
@@ -533,8 +593,11 @@
       <c r="C9" s="1">
         <v>55</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -544,8 +607,11 @@
       <c r="C10" s="1">
         <v>25</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -555,8 +621,11 @@
       <c r="C11" s="1">
         <v>60</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
@@ -566,8 +635,11 @@
       <c r="C12" s="1">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -577,8 +649,11 @@
       <c r="C13" s="1">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -588,8 +663,11 @@
       <c r="C14" s="1">
         <v>46</v>
       </c>
-    </row>
-    <row r="15" spans="1:3">
+      <c r="D14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -599,8 +677,11 @@
       <c r="C15" s="1">
         <v>77</v>
       </c>
-    </row>
-    <row r="16" spans="1:3">
+      <c r="D15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
@@ -610,8 +691,11 @@
       <c r="C16" s="1">
         <v>34</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,8 +705,11 @@
       <c r="C17" s="1">
         <v>56</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -632,8 +719,11 @@
       <c r="C18" s="1">
         <v>76</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -643,9 +733,13 @@
       <c r="C19" s="1">
         <v>40</v>
       </c>
+      <c r="D19">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -655,10 +749,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="26" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.26953125" customWidth="1"/>
+    <col min="2" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="14.25" customHeight="1">
@@ -1693,13 +1787,15 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1709,8 +1805,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1720,8 +1819,11 @@
       <c r="C2" s="1">
         <v>150</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1731,8 +1833,11 @@
       <c r="C3" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -1742,8 +1847,11 @@
       <c r="C4" s="1">
         <v>100</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -1753,8 +1861,11 @@
       <c r="C5" s="1">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1764,8 +1875,11 @@
       <c r="C6" s="1">
         <v>125</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -1774,6 +1888,9 @@
       </c>
       <c r="C7" s="1">
         <v>130</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -1788,9 +1905,11 @@
   </sheetPr>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -2015,7 +2134,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="7" t="s">
@@ -2052,4 +2171,69 @@
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C942FF0-AAA4-4139-9946-71CCFDA35845}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="11">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="11">
+        <v>0.3</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="11">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>